<commit_message>
Vladimiro ir Tomos dienynai
</commit_message>
<xml_diff>
--- a/Dienynas JAVA 0605.xlsx
+++ b/Dienynas JAVA 0605.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="12960" windowHeight="6300" tabRatio="836" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="12960" windowHeight="6300" tabRatio="836"/>
   </bookViews>
   <sheets>
     <sheet name="1. Tarnyb. stotys" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="858" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="206">
   <si>
     <t>mėnuo / diena</t>
   </si>
@@ -953,6 +953,8 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -971,8 +973,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
@@ -1277,7 +1277,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
@@ -1364,10 +1364,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="39" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -1419,25 +1419,25 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="39" t="s">
+      <c r="AB3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="35" t="s">
+      <c r="AC3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="35" t="s">
+      <c r="AD3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="35" t="s">
+      <c r="AE3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="35" t="s">
+      <c r="AF3" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="38"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="15" t="s">
         <v>102</v>
       </c>
@@ -1487,11 +1487,11 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="36"/>
-      <c r="AF4" s="36"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
     </row>
     <row r="5" spans="1:32" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="28">
@@ -2111,7 +2111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
@@ -2199,10 +2199,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="39" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="14" t="s">
@@ -2252,25 +2252,25 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="39" t="s">
+      <c r="AB3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="35" t="s">
+      <c r="AC3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="35" t="s">
+      <c r="AD3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="35" t="s">
+      <c r="AE3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="35" t="s">
+      <c r="AF3" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="38"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="14" t="s">
         <v>61</v>
       </c>
@@ -2318,11 +2318,11 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="36"/>
-      <c r="AF4" s="36"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
     </row>
     <row r="5" spans="1:32" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="24">
@@ -2984,10 +2984,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="39" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -3041,25 +3041,25 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="35" t="s">
+      <c r="AB3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="35" t="s">
+      <c r="AC3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="35" t="s">
+      <c r="AD3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="35" t="s">
+      <c r="AE3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="35" t="s">
+      <c r="AF3" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="15" t="s">
         <v>77</v>
       </c>
@@ -3111,11 +3111,11 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="36"/>
-      <c r="AF4" s="36"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
     </row>
     <row r="5" spans="1:32" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -3824,10 +3824,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="39" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="33" t="s">
@@ -3899,25 +3899,25 @@
       <c r="Y3" s="33"/>
       <c r="Z3" s="33"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="35" t="s">
+      <c r="AB3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="35" t="s">
+      <c r="AC3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="35" t="s">
+      <c r="AD3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="35" t="s">
+      <c r="AE3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="35" t="s">
+      <c r="AF3" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="9">
         <v>12</v>
       </c>
@@ -3987,11 +3987,11 @@
       <c r="Y4" s="33"/>
       <c r="Z4" s="33"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="36"/>
-      <c r="AF4" s="36"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
     </row>
     <row r="5" spans="1:32" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -5017,7 +5017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
@@ -5104,10 +5104,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="39" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="33" t="s">
@@ -5157,25 +5157,25 @@
       <c r="Y3" s="9"/>
       <c r="Z3" s="9"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="35" t="s">
+      <c r="AB3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="35" t="s">
+      <c r="AC3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="35" t="s">
+      <c r="AD3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="35" t="s">
+      <c r="AE3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="35" t="s">
+      <c r="AF3" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="33" t="s">
         <v>72</v>
       </c>
@@ -5223,11 +5223,11 @@
       <c r="Y4" s="9"/>
       <c r="Z4" s="9"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="36"/>
-      <c r="AF4" s="36"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
     </row>
     <row r="5" spans="1:32" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -5763,7 +5763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AB17" sqref="AB17"/>
     </sheetView>
   </sheetViews>
@@ -5850,10 +5850,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="39" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -5905,25 +5905,25 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="35" t="s">
+      <c r="AB3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="35" t="s">
+      <c r="AC3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="35" t="s">
+      <c r="AD3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="35" t="s">
+      <c r="AE3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="35" t="s">
+      <c r="AF3" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="15" t="s">
         <v>98</v>
       </c>
@@ -5973,11 +5973,11 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="36"/>
-      <c r="AF4" s="36"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
     </row>
     <row r="5" spans="1:32" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -6643,10 +6643,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="39" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -6716,25 +6716,25 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="39" t="s">
+      <c r="AB3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="35" t="s">
+      <c r="AC3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="35" t="s">
+      <c r="AD3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="35" t="s">
+      <c r="AE3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="35" t="s">
+      <c r="AF3" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="15" t="s">
         <v>63</v>
       </c>
@@ -6802,11 +6802,11 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="40"/>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="36"/>
-      <c r="AF4" s="36"/>
+      <c r="AB4" s="42"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
     </row>
     <row r="5" spans="1:32" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -7854,8 +7854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7941,10 +7941,10 @@
       <c r="AF2" s="5"/>
     </row>
     <row r="3" spans="1:32" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="39" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="15" t="s">
@@ -7954,7 +7954,7 @@
         <v>75</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F3" s="15" t="s">
         <v>76</v>
@@ -7977,7 +7977,9 @@
       <c r="L3" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="M3" s="15"/>
+      <c r="M3" s="15" t="s">
+        <v>76</v>
+      </c>
       <c r="N3" s="15"/>
       <c r="O3" s="15"/>
       <c r="P3" s="15"/>
@@ -7992,56 +7994,58 @@
       <c r="Y3" s="15"/>
       <c r="Z3" s="15"/>
       <c r="AA3" s="1"/>
-      <c r="AB3" s="35" t="s">
+      <c r="AB3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="35" t="s">
+      <c r="AC3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AD3" s="35" t="s">
+      <c r="AD3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="AE3" s="35" t="s">
+      <c r="AE3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="35" t="s">
+      <c r="AF3" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="E4" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="F4" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="G4" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="H4" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="I4" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="J4" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="K4" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="L4" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="M4" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="M4" s="15"/>
       <c r="N4" s="15"/>
       <c r="O4" s="15"/>
       <c r="P4" s="15"/>
@@ -8056,11 +8060,11 @@
       <c r="Y4" s="15"/>
       <c r="Z4" s="15"/>
       <c r="AA4" s="1"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="36"/>
-      <c r="AF4" s="36"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
     </row>
     <row r="5" spans="1:32" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
@@ -8099,7 +8103,9 @@
       <c r="L5" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="M5" s="10"/>
+      <c r="M5" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
       <c r="P5" s="10"/>
@@ -8624,13 +8630,13 @@
       <c r="N2" t="s">
         <v>159</v>
       </c>
-      <c r="O2" s="42">
+      <c r="O2" s="36">
         <v>2</v>
       </c>
       <c r="Q2" t="s">
         <v>180</v>
       </c>
-      <c r="R2" s="41">
+      <c r="R2" s="35">
         <v>7</v>
       </c>
     </row>
@@ -8662,13 +8668,13 @@
       <c r="N3" t="s">
         <v>160</v>
       </c>
-      <c r="O3" s="42">
+      <c r="O3" s="36">
         <v>2</v>
       </c>
       <c r="Q3" t="s">
         <v>181</v>
       </c>
-      <c r="R3" s="41"/>
+      <c r="R3" s="35"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -8698,13 +8704,13 @@
       <c r="N4" t="s">
         <v>161</v>
       </c>
-      <c r="O4" s="42">
+      <c r="O4" s="36">
         <v>2</v>
       </c>
       <c r="Q4" t="s">
         <v>182</v>
       </c>
-      <c r="R4" s="41"/>
+      <c r="R4" s="35"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
@@ -8734,13 +8740,13 @@
       <c r="N5" t="s">
         <v>162</v>
       </c>
-      <c r="O5" s="42">
+      <c r="O5" s="36">
         <v>3</v>
       </c>
       <c r="Q5" t="s">
         <v>183</v>
       </c>
-      <c r="R5" s="41"/>
+      <c r="R5" s="35"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -8770,13 +8776,13 @@
       <c r="N6" t="s">
         <v>163</v>
       </c>
-      <c r="O6" s="42">
+      <c r="O6" s="36">
         <v>3</v>
       </c>
       <c r="Q6" t="s">
         <v>184</v>
       </c>
-      <c r="R6" s="41">
+      <c r="R6" s="35">
         <v>7</v>
       </c>
     </row>
@@ -8808,13 +8814,13 @@
       <c r="N7" t="s">
         <v>164</v>
       </c>
-      <c r="O7" s="42">
+      <c r="O7" s="36">
         <v>3</v>
       </c>
       <c r="Q7" t="s">
         <v>185</v>
       </c>
-      <c r="R7" s="41">
+      <c r="R7" s="35">
         <v>7</v>
       </c>
     </row>
@@ -8846,13 +8852,13 @@
       <c r="N8" t="s">
         <v>165</v>
       </c>
-      <c r="O8" s="42">
+      <c r="O8" s="36">
         <v>3</v>
       </c>
       <c r="Q8" t="s">
         <v>186</v>
       </c>
-      <c r="R8" s="41">
+      <c r="R8" s="35">
         <v>7</v>
       </c>
     </row>
@@ -8884,13 +8890,13 @@
       <c r="N9" t="s">
         <v>166</v>
       </c>
-      <c r="O9" s="42">
+      <c r="O9" s="36">
         <v>3</v>
       </c>
       <c r="Q9" t="s">
         <v>187</v>
       </c>
-      <c r="R9" s="41">
+      <c r="R9" s="35">
         <v>7</v>
       </c>
     </row>
@@ -8922,13 +8928,13 @@
       <c r="N10" t="s">
         <v>167</v>
       </c>
-      <c r="O10" s="42">
+      <c r="O10" s="36">
         <v>3</v>
       </c>
       <c r="Q10" t="s">
         <v>188</v>
       </c>
-      <c r="R10" s="41">
+      <c r="R10" s="35">
         <v>7</v>
       </c>
     </row>
@@ -8960,13 +8966,13 @@
       <c r="N11" t="s">
         <v>168</v>
       </c>
-      <c r="O11" s="42">
+      <c r="O11" s="36">
         <v>3</v>
       </c>
       <c r="Q11" t="s">
         <v>189</v>
       </c>
-      <c r="R11" s="41">
+      <c r="R11" s="35">
         <v>7</v>
       </c>
     </row>
@@ -8998,13 +9004,13 @@
       <c r="N12" t="s">
         <v>169</v>
       </c>
-      <c r="O12" s="42">
+      <c r="O12" s="36">
         <v>3</v>
       </c>
       <c r="Q12" t="s">
         <v>190</v>
       </c>
-      <c r="R12" s="41">
+      <c r="R12" s="35">
         <v>7</v>
       </c>
     </row>
@@ -9036,13 +9042,13 @@
       <c r="N13" t="s">
         <v>171</v>
       </c>
-      <c r="O13" s="42">
+      <c r="O13" s="36">
         <v>3</v>
       </c>
       <c r="Q13" t="s">
         <v>191</v>
       </c>
-      <c r="R13" s="41">
+      <c r="R13" s="35">
         <v>8</v>
       </c>
     </row>
@@ -9074,7 +9080,7 @@
       <c r="N14" t="s">
         <v>172</v>
       </c>
-      <c r="O14" s="42">
+      <c r="O14" s="36">
         <v>3</v>
       </c>
     </row>
@@ -9100,13 +9106,13 @@
       <c r="K15" t="s">
         <v>154</v>
       </c>
-      <c r="L15" s="42">
+      <c r="L15" s="36">
         <v>4</v>
       </c>
       <c r="N15" t="s">
         <v>174</v>
       </c>
-      <c r="O15" s="42">
+      <c r="O15" s="36">
         <v>3</v>
       </c>
     </row>
@@ -9132,13 +9138,13 @@
       <c r="K16" t="s">
         <v>155</v>
       </c>
-      <c r="L16" s="42">
+      <c r="L16" s="36">
         <v>4</v>
       </c>
       <c r="N16" t="s">
         <v>204</v>
       </c>
-      <c r="O16" s="41">
+      <c r="O16" s="35">
         <v>7</v>
       </c>
     </row>
@@ -9164,13 +9170,13 @@
       <c r="K17" t="s">
         <v>156</v>
       </c>
-      <c r="L17" s="42">
+      <c r="L17" s="36">
         <v>4</v>
       </c>
       <c r="N17" t="s">
         <v>175</v>
       </c>
-      <c r="O17" s="41">
+      <c r="O17" s="35">
         <v>7</v>
       </c>
     </row>
@@ -9196,13 +9202,13 @@
       <c r="K18" t="s">
         <v>157</v>
       </c>
-      <c r="L18" s="42">
+      <c r="L18" s="36">
         <v>2</v>
       </c>
       <c r="N18" t="s">
         <v>176</v>
       </c>
-      <c r="O18" s="41">
+      <c r="O18" s="35">
         <v>7</v>
       </c>
     </row>
@@ -9228,13 +9234,13 @@
       <c r="K19" t="s">
         <v>202</v>
       </c>
-      <c r="L19" s="42">
+      <c r="L19" s="36">
         <v>2</v>
       </c>
       <c r="N19" t="s">
         <v>177</v>
       </c>
-      <c r="O19" s="41">
+      <c r="O19" s="35">
         <v>7</v>
       </c>
     </row>
@@ -9260,13 +9266,13 @@
       <c r="K20" t="s">
         <v>158</v>
       </c>
-      <c r="L20" s="42">
+      <c r="L20" s="36">
         <v>2</v>
       </c>
       <c r="N20" t="s">
         <v>178</v>
       </c>
-      <c r="O20" s="41">
+      <c r="O20" s="35">
         <v>7</v>
       </c>
     </row>
@@ -9286,13 +9292,13 @@
       <c r="K21" t="s">
         <v>203</v>
       </c>
-      <c r="L21" s="42">
+      <c r="L21" s="36">
         <v>2</v>
       </c>
       <c r="N21" t="s">
         <v>179</v>
       </c>
-      <c r="O21" s="41">
+      <c r="O21" s="35">
         <v>7</v>
       </c>
     </row>

</xml_diff>